<commit_message>
Fill pivot table shared items from records.
Shared item contain unique items from each data field and
they weren't correctly filled refresh. It caused writer to write incorrect
indexes to shared items in pivotField attribute. That caused corrupted file.

Change shared items as a full structure, that is updated in sync with cache records
(except when loading) and use it's actual values during saving. Originally, there was
distinct that caused invalid references.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/TwoPivotTablesWithSingleSource/output.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/TwoPivotTablesWithSingleSource/output.xlsx
@@ -1291,2311 +1291,649 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" itemPrintTitles="1" mergeItem="1" indent="0" compact="0" compactData="0" gridDropZones="1">
-  <x:location ref="B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="7">
-    <x:pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="55">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item x="7"/>
-        <x:item x="8"/>
-        <x:item x="9"/>
-        <x:item x="10"/>
-        <x:item x="11"/>
-        <x:item x="12"/>
-        <x:item x="13"/>
-        <x:item x="14"/>
-        <x:item x="15"/>
-        <x:item x="16"/>
-        <x:item x="17"/>
-        <x:item x="18"/>
-        <x:item x="19"/>
-        <x:item x="20"/>
-        <x:item x="21"/>
-        <x:item x="22"/>
-        <x:item x="23"/>
-        <x:item x="24"/>
-        <x:item x="25"/>
-        <x:item x="26"/>
-        <x:item x="27"/>
-        <x:item x="28"/>
-        <x:item x="29"/>
-        <x:item x="30"/>
-        <x:item x="31"/>
-        <x:item x="32"/>
-        <x:item x="33"/>
-        <x:item x="34"/>
-        <x:item x="35"/>
-        <x:item x="36"/>
-        <x:item x="37"/>
-        <x:item x="38"/>
-        <x:item x="39"/>
-        <x:item x="40"/>
-        <x:item x="41"/>
-        <x:item x="42"/>
-        <x:item x="43"/>
-        <x:item x="44"/>
-        <x:item x="45"/>
-        <x:item x="46"/>
-        <x:item x="47"/>
-        <x:item x="48"/>
-        <x:item x="49"/>
-        <x:item x="50"/>
-        <x:item x="51"/>
-        <x:item x="52"/>
-        <x:item x="53"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Payment method" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="8">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="206">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item x="7"/>
-        <x:item x="8"/>
-        <x:item x="9"/>
-        <x:item x="10"/>
-        <x:item x="11"/>
-        <x:item x="12"/>
-        <x:item x="13"/>
-        <x:item x="14"/>
-        <x:item x="15"/>
-        <x:item x="16"/>
-        <x:item x="17"/>
-        <x:item x="18"/>
-        <x:item x="19"/>
-        <x:item x="20"/>
-        <x:item x="21"/>
-        <x:item x="22"/>
-        <x:item x="23"/>
-        <x:item x="24"/>
-        <x:item x="25"/>
-        <x:item x="26"/>
-        <x:item x="27"/>
-        <x:item x="28"/>
-        <x:item x="29"/>
-        <x:item x="30"/>
-        <x:item x="31"/>
-        <x:item x="32"/>
-        <x:item x="33"/>
-        <x:item x="34"/>
-        <x:item x="35"/>
-        <x:item x="36"/>
-        <x:item x="37"/>
-        <x:item x="38"/>
-        <x:item x="39"/>
-        <x:item x="40"/>
-        <x:item x="41"/>
-        <x:item x="42"/>
-        <x:item x="43"/>
-        <x:item x="44"/>
-        <x:item x="45"/>
-        <x:item x="46"/>
-        <x:item x="47"/>
-        <x:item x="48"/>
-        <x:item x="49"/>
-        <x:item x="50"/>
-        <x:item x="51"/>
-        <x:item x="52"/>
-        <x:item x="53"/>
-        <x:item x="54"/>
-        <x:item x="55"/>
-        <x:item x="56"/>
-        <x:item x="57"/>
-        <x:item x="58"/>
-        <x:item x="59"/>
-        <x:item x="60"/>
-        <x:item x="61"/>
-        <x:item x="62"/>
-        <x:item x="63"/>
-        <x:item x="64"/>
-        <x:item x="65"/>
-        <x:item x="66"/>
-        <x:item x="67"/>
-        <x:item x="68"/>
-        <x:item x="69"/>
-        <x:item x="70"/>
-        <x:item x="71"/>
-        <x:item x="72"/>
-        <x:item x="73"/>
-        <x:item x="74"/>
-        <x:item x="75"/>
-        <x:item x="76"/>
-        <x:item x="77"/>
-        <x:item x="78"/>
-        <x:item x="79"/>
-        <x:item x="80"/>
-        <x:item x="81"/>
-        <x:item x="82"/>
-        <x:item x="83"/>
-        <x:item x="84"/>
-        <x:item x="85"/>
-        <x:item x="86"/>
-        <x:item x="87"/>
-        <x:item x="88"/>
-        <x:item x="89"/>
-        <x:item x="90"/>
-        <x:item x="91"/>
-        <x:item x="92"/>
-        <x:item x="93"/>
-        <x:item x="94"/>
-        <x:item x="95"/>
-        <x:item x="96"/>
-        <x:item x="97"/>
-        <x:item x="98"/>
-        <x:item x="99"/>
-        <x:item x="100"/>
-        <x:item x="101"/>
-        <x:item x="102"/>
-        <x:item x="103"/>
-        <x:item x="104"/>
-        <x:item x="105"/>
-        <x:item x="106"/>
-        <x:item x="107"/>
-        <x:item x="108"/>
-        <x:item x="109"/>
-        <x:item x="110"/>
-        <x:item x="111"/>
-        <x:item x="112"/>
-        <x:item x="113"/>
-        <x:item x="114"/>
-        <x:item x="115"/>
-        <x:item x="116"/>
-        <x:item x="117"/>
-        <x:item x="118"/>
-        <x:item x="119"/>
-        <x:item x="120"/>
-        <x:item x="121"/>
-        <x:item x="122"/>
-        <x:item x="123"/>
-        <x:item x="124"/>
-        <x:item x="125"/>
-        <x:item x="126"/>
-        <x:item x="127"/>
-        <x:item x="128"/>
-        <x:item x="129"/>
-        <x:item x="130"/>
-        <x:item x="131"/>
-        <x:item x="132"/>
-        <x:item x="133"/>
-        <x:item x="134"/>
-        <x:item x="135"/>
-        <x:item x="136"/>
-        <x:item x="137"/>
-        <x:item x="138"/>
-        <x:item x="139"/>
-        <x:item x="140"/>
-        <x:item x="141"/>
-        <x:item x="142"/>
-        <x:item x="143"/>
-        <x:item x="144"/>
-        <x:item x="145"/>
-        <x:item x="146"/>
-        <x:item x="147"/>
-        <x:item x="148"/>
-        <x:item x="149"/>
-        <x:item x="150"/>
-        <x:item x="151"/>
-        <x:item x="152"/>
-        <x:item x="153"/>
-        <x:item x="154"/>
-        <x:item x="155"/>
-        <x:item x="156"/>
-        <x:item x="157"/>
-        <x:item x="158"/>
-        <x:item x="159"/>
-        <x:item x="160"/>
-        <x:item x="161"/>
-        <x:item x="162"/>
-        <x:item x="163"/>
-        <x:item x="164"/>
-        <x:item x="165"/>
-        <x:item x="166"/>
-        <x:item x="167"/>
-        <x:item x="168"/>
-        <x:item x="169"/>
-        <x:item x="170"/>
-        <x:item x="171"/>
-        <x:item x="172"/>
-        <x:item x="173"/>
-        <x:item x="174"/>
-        <x:item x="175"/>
-        <x:item x="176"/>
-        <x:item x="177"/>
-        <x:item x="178"/>
-        <x:item x="179"/>
-        <x:item x="180"/>
-        <x:item x="181"/>
-        <x:item x="182"/>
-        <x:item x="183"/>
-        <x:item x="184"/>
-        <x:item x="185"/>
-        <x:item x="186"/>
-        <x:item x="187"/>
-        <x:item x="188"/>
-        <x:item x="189"/>
-        <x:item x="190"/>
-        <x:item x="191"/>
-        <x:item x="192"/>
-        <x:item x="193"/>
-        <x:item x="194"/>
-        <x:item x="195"/>
-        <x:item x="196"/>
-        <x:item x="197"/>
-        <x:item x="198"/>
-        <x:item x="199"/>
-        <x:item x="200"/>
-        <x:item x="201"/>
-        <x:item x="202"/>
-        <x:item x="203"/>
-        <x:item x="204"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Ship date" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Items total" dataField="1" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Tax rate" axis="axisCol" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="4">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Amount paid" dataField="1" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-  </x:pivotFields>
-  <x:rowFields count="3">
-    <x:field x="0"/>
-    <x:field x="1"/>
-    <x:field x="2"/>
-  </x:rowFields>
-  <x:rowItems count="269">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i>
-      <x:x v="5"/>
-    </x:i>
-    <x:i>
-      <x:x v="6"/>
-    </x:i>
-    <x:i>
-      <x:x v="7"/>
-    </x:i>
-    <x:i>
-      <x:x v="8"/>
-    </x:i>
-    <x:i>
-      <x:x v="9"/>
-    </x:i>
-    <x:i>
-      <x:x v="10"/>
-    </x:i>
-    <x:i>
-      <x:x v="11"/>
-    </x:i>
-    <x:i>
-      <x:x v="12"/>
-    </x:i>
-    <x:i>
-      <x:x v="13"/>
-    </x:i>
-    <x:i>
-      <x:x v="14"/>
-    </x:i>
-    <x:i>
-      <x:x v="15"/>
-    </x:i>
-    <x:i>
-      <x:x v="16"/>
-    </x:i>
-    <x:i>
-      <x:x v="17"/>
-    </x:i>
-    <x:i>
-      <x:x v="18"/>
-    </x:i>
-    <x:i>
-      <x:x v="19"/>
-    </x:i>
-    <x:i>
-      <x:x v="20"/>
-    </x:i>
-    <x:i>
-      <x:x v="21"/>
-    </x:i>
-    <x:i>
-      <x:x v="22"/>
-    </x:i>
-    <x:i>
-      <x:x v="23"/>
-    </x:i>
-    <x:i>
-      <x:x v="24"/>
-    </x:i>
-    <x:i>
-      <x:x v="25"/>
-    </x:i>
-    <x:i>
-      <x:x v="26"/>
-    </x:i>
-    <x:i>
-      <x:x v="27"/>
-    </x:i>
-    <x:i>
-      <x:x v="28"/>
-    </x:i>
-    <x:i>
-      <x:x v="29"/>
-    </x:i>
-    <x:i>
-      <x:x v="30"/>
-    </x:i>
-    <x:i>
-      <x:x v="31"/>
-    </x:i>
-    <x:i>
-      <x:x v="32"/>
-    </x:i>
-    <x:i>
-      <x:x v="33"/>
-    </x:i>
-    <x:i>
-      <x:x v="34"/>
-    </x:i>
-    <x:i>
-      <x:x v="35"/>
-    </x:i>
-    <x:i>
-      <x:x v="36"/>
-    </x:i>
-    <x:i>
-      <x:x v="37"/>
-    </x:i>
-    <x:i>
-      <x:x v="38"/>
-    </x:i>
-    <x:i>
-      <x:x v="39"/>
-    </x:i>
-    <x:i>
-      <x:x v="40"/>
-    </x:i>
-    <x:i>
-      <x:x v="41"/>
-    </x:i>
-    <x:i>
-      <x:x v="42"/>
-    </x:i>
-    <x:i>
-      <x:x v="43"/>
-    </x:i>
-    <x:i>
-      <x:x v="44"/>
-    </x:i>
-    <x:i>
-      <x:x v="45"/>
-    </x:i>
-    <x:i>
-      <x:x v="46"/>
-    </x:i>
-    <x:i>
-      <x:x v="47"/>
-    </x:i>
-    <x:i>
-      <x:x v="48"/>
-    </x:i>
-    <x:i>
-      <x:x v="49"/>
-    </x:i>
-    <x:i>
-      <x:x v="50"/>
-    </x:i>
-    <x:i>
-      <x:x v="51"/>
-    </x:i>
-    <x:i>
-      <x:x v="52"/>
-    </x:i>
-    <x:i>
-      <x:x v="53"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i>
-      <x:x v="5"/>
-    </x:i>
-    <x:i>
-      <x:x v="6"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i>
-      <x:x v="5"/>
-    </x:i>
-    <x:i>
-      <x:x v="6"/>
-    </x:i>
-    <x:i>
-      <x:x v="7"/>
-    </x:i>
-    <x:i>
-      <x:x v="8"/>
-    </x:i>
-    <x:i>
-      <x:x v="9"/>
-    </x:i>
-    <x:i>
-      <x:x v="10"/>
-    </x:i>
-    <x:i>
-      <x:x v="11"/>
-    </x:i>
-    <x:i>
-      <x:x v="12"/>
-    </x:i>
-    <x:i>
-      <x:x v="13"/>
-    </x:i>
-    <x:i>
-      <x:x v="14"/>
-    </x:i>
-    <x:i>
-      <x:x v="15"/>
-    </x:i>
-    <x:i>
-      <x:x v="16"/>
-    </x:i>
-    <x:i>
-      <x:x v="17"/>
-    </x:i>
-    <x:i>
-      <x:x v="18"/>
-    </x:i>
-    <x:i>
-      <x:x v="19"/>
-    </x:i>
-    <x:i>
-      <x:x v="20"/>
-    </x:i>
-    <x:i>
-      <x:x v="21"/>
-    </x:i>
-    <x:i>
-      <x:x v="22"/>
-    </x:i>
-    <x:i>
-      <x:x v="23"/>
-    </x:i>
-    <x:i>
-      <x:x v="24"/>
-    </x:i>
-    <x:i>
-      <x:x v="25"/>
-    </x:i>
-    <x:i>
-      <x:x v="26"/>
-    </x:i>
-    <x:i>
-      <x:x v="27"/>
-    </x:i>
-    <x:i>
-      <x:x v="28"/>
-    </x:i>
-    <x:i>
-      <x:x v="29"/>
-    </x:i>
-    <x:i>
-      <x:x v="30"/>
-    </x:i>
-    <x:i>
-      <x:x v="31"/>
-    </x:i>
-    <x:i>
-      <x:x v="32"/>
-    </x:i>
-    <x:i>
-      <x:x v="33"/>
-    </x:i>
-    <x:i>
-      <x:x v="34"/>
-    </x:i>
-    <x:i>
-      <x:x v="35"/>
-    </x:i>
-    <x:i>
-      <x:x v="36"/>
-    </x:i>
-    <x:i>
-      <x:x v="37"/>
-    </x:i>
-    <x:i>
-      <x:x v="38"/>
-    </x:i>
-    <x:i>
-      <x:x v="39"/>
-    </x:i>
-    <x:i>
-      <x:x v="40"/>
-    </x:i>
-    <x:i>
-      <x:x v="41"/>
-    </x:i>
-    <x:i>
-      <x:x v="42"/>
-    </x:i>
-    <x:i>
-      <x:x v="43"/>
-    </x:i>
-    <x:i>
-      <x:x v="44"/>
-    </x:i>
-    <x:i>
-      <x:x v="45"/>
-    </x:i>
-    <x:i>
-      <x:x v="46"/>
-    </x:i>
-    <x:i>
-      <x:x v="47"/>
-    </x:i>
-    <x:i>
-      <x:x v="48"/>
-    </x:i>
-    <x:i>
-      <x:x v="49"/>
-    </x:i>
-    <x:i>
-      <x:x v="50"/>
-    </x:i>
-    <x:i>
-      <x:x v="51"/>
-    </x:i>
-    <x:i>
-      <x:x v="52"/>
-    </x:i>
-    <x:i>
-      <x:x v="53"/>
-    </x:i>
-    <x:i>
-      <x:x v="54"/>
-    </x:i>
-    <x:i>
-      <x:x v="55"/>
-    </x:i>
-    <x:i>
-      <x:x v="56"/>
-    </x:i>
-    <x:i>
-      <x:x v="57"/>
-    </x:i>
-    <x:i>
-      <x:x v="58"/>
-    </x:i>
-    <x:i>
-      <x:x v="59"/>
-    </x:i>
-    <x:i>
-      <x:x v="60"/>
-    </x:i>
-    <x:i>
-      <x:x v="61"/>
-    </x:i>
-    <x:i>
-      <x:x v="62"/>
-    </x:i>
-    <x:i>
-      <x:x v="63"/>
-    </x:i>
-    <x:i>
-      <x:x v="64"/>
-    </x:i>
-    <x:i>
-      <x:x v="65"/>
-    </x:i>
-    <x:i>
-      <x:x v="66"/>
-    </x:i>
-    <x:i>
-      <x:x v="67"/>
-    </x:i>
-    <x:i>
-      <x:x v="68"/>
-    </x:i>
-    <x:i>
-      <x:x v="69"/>
-    </x:i>
-    <x:i>
-      <x:x v="70"/>
-    </x:i>
-    <x:i>
-      <x:x v="71"/>
-    </x:i>
-    <x:i>
-      <x:x v="72"/>
-    </x:i>
-    <x:i>
-      <x:x v="73"/>
-    </x:i>
-    <x:i>
-      <x:x v="74"/>
-    </x:i>
-    <x:i>
-      <x:x v="75"/>
-    </x:i>
-    <x:i>
-      <x:x v="76"/>
-    </x:i>
-    <x:i>
-      <x:x v="77"/>
-    </x:i>
-    <x:i>
-      <x:x v="78"/>
-    </x:i>
-    <x:i>
-      <x:x v="79"/>
-    </x:i>
-    <x:i>
-      <x:x v="80"/>
-    </x:i>
-    <x:i>
-      <x:x v="81"/>
-    </x:i>
-    <x:i>
-      <x:x v="82"/>
-    </x:i>
-    <x:i>
-      <x:x v="83"/>
-    </x:i>
-    <x:i>
-      <x:x v="84"/>
-    </x:i>
-    <x:i>
-      <x:x v="85"/>
-    </x:i>
-    <x:i>
-      <x:x v="86"/>
-    </x:i>
-    <x:i>
-      <x:x v="87"/>
-    </x:i>
-    <x:i>
-      <x:x v="88"/>
-    </x:i>
-    <x:i>
-      <x:x v="89"/>
-    </x:i>
-    <x:i>
-      <x:x v="90"/>
-    </x:i>
-    <x:i>
-      <x:x v="91"/>
-    </x:i>
-    <x:i>
-      <x:x v="92"/>
-    </x:i>
-    <x:i>
-      <x:x v="93"/>
-    </x:i>
-    <x:i>
-      <x:x v="94"/>
-    </x:i>
-    <x:i>
-      <x:x v="95"/>
-    </x:i>
-    <x:i>
-      <x:x v="96"/>
-    </x:i>
-    <x:i>
-      <x:x v="97"/>
-    </x:i>
-    <x:i>
-      <x:x v="98"/>
-    </x:i>
-    <x:i>
-      <x:x v="99"/>
-    </x:i>
-    <x:i>
-      <x:x v="100"/>
-    </x:i>
-    <x:i>
-      <x:x v="101"/>
-    </x:i>
-    <x:i>
-      <x:x v="102"/>
-    </x:i>
-    <x:i>
-      <x:x v="103"/>
-    </x:i>
-    <x:i>
-      <x:x v="104"/>
-    </x:i>
-    <x:i>
-      <x:x v="105"/>
-    </x:i>
-    <x:i>
-      <x:x v="106"/>
-    </x:i>
-    <x:i>
-      <x:x v="107"/>
-    </x:i>
-    <x:i>
-      <x:x v="108"/>
-    </x:i>
-    <x:i>
-      <x:x v="109"/>
-    </x:i>
-    <x:i>
-      <x:x v="110"/>
-    </x:i>
-    <x:i>
-      <x:x v="111"/>
-    </x:i>
-    <x:i>
-      <x:x v="112"/>
-    </x:i>
-    <x:i>
-      <x:x v="113"/>
-    </x:i>
-    <x:i>
-      <x:x v="114"/>
-    </x:i>
-    <x:i>
-      <x:x v="115"/>
-    </x:i>
-    <x:i>
-      <x:x v="116"/>
-    </x:i>
-    <x:i>
-      <x:x v="117"/>
-    </x:i>
-    <x:i>
-      <x:x v="118"/>
-    </x:i>
-    <x:i>
-      <x:x v="119"/>
-    </x:i>
-    <x:i>
-      <x:x v="120"/>
-    </x:i>
-    <x:i>
-      <x:x v="121"/>
-    </x:i>
-    <x:i>
-      <x:x v="122"/>
-    </x:i>
-    <x:i>
-      <x:x v="123"/>
-    </x:i>
-    <x:i>
-      <x:x v="124"/>
-    </x:i>
-    <x:i>
-      <x:x v="125"/>
-    </x:i>
-    <x:i>
-      <x:x v="126"/>
-    </x:i>
-    <x:i>
-      <x:x v="127"/>
-    </x:i>
-    <x:i>
-      <x:x v="128"/>
-    </x:i>
-    <x:i>
-      <x:x v="129"/>
-    </x:i>
-    <x:i>
-      <x:x v="130"/>
-    </x:i>
-    <x:i>
-      <x:x v="131"/>
-    </x:i>
-    <x:i>
-      <x:x v="132"/>
-    </x:i>
-    <x:i>
-      <x:x v="133"/>
-    </x:i>
-    <x:i>
-      <x:x v="134"/>
-    </x:i>
-    <x:i>
-      <x:x v="135"/>
-    </x:i>
-    <x:i>
-      <x:x v="136"/>
-    </x:i>
-    <x:i>
-      <x:x v="137"/>
-    </x:i>
-    <x:i>
-      <x:x v="138"/>
-    </x:i>
-    <x:i>
-      <x:x v="139"/>
-    </x:i>
-    <x:i>
-      <x:x v="140"/>
-    </x:i>
-    <x:i>
-      <x:x v="141"/>
-    </x:i>
-    <x:i>
-      <x:x v="142"/>
-    </x:i>
-    <x:i>
-      <x:x v="143"/>
-    </x:i>
-    <x:i>
-      <x:x v="144"/>
-    </x:i>
-    <x:i>
-      <x:x v="145"/>
-    </x:i>
-    <x:i>
-      <x:x v="146"/>
-    </x:i>
-    <x:i>
-      <x:x v="147"/>
-    </x:i>
-    <x:i>
-      <x:x v="148"/>
-    </x:i>
-    <x:i>
-      <x:x v="149"/>
-    </x:i>
-    <x:i>
-      <x:x v="150"/>
-    </x:i>
-    <x:i>
-      <x:x v="151"/>
-    </x:i>
-    <x:i>
-      <x:x v="152"/>
-    </x:i>
-    <x:i>
-      <x:x v="153"/>
-    </x:i>
-    <x:i>
-      <x:x v="154"/>
-    </x:i>
-    <x:i>
-      <x:x v="155"/>
-    </x:i>
-    <x:i>
-      <x:x v="156"/>
-    </x:i>
-    <x:i>
-      <x:x v="157"/>
-    </x:i>
-    <x:i>
-      <x:x v="158"/>
-    </x:i>
-    <x:i>
-      <x:x v="159"/>
-    </x:i>
-    <x:i>
-      <x:x v="160"/>
-    </x:i>
-    <x:i>
-      <x:x v="161"/>
-    </x:i>
-    <x:i>
-      <x:x v="162"/>
-    </x:i>
-    <x:i>
-      <x:x v="163"/>
-    </x:i>
-    <x:i>
-      <x:x v="164"/>
-    </x:i>
-    <x:i>
-      <x:x v="165"/>
-    </x:i>
-    <x:i>
-      <x:x v="166"/>
-    </x:i>
-    <x:i>
-      <x:x v="167"/>
-    </x:i>
-    <x:i>
-      <x:x v="168"/>
-    </x:i>
-    <x:i>
-      <x:x v="169"/>
-    </x:i>
-    <x:i>
-      <x:x v="170"/>
-    </x:i>
-    <x:i>
-      <x:x v="171"/>
-    </x:i>
-    <x:i>
-      <x:x v="172"/>
-    </x:i>
-    <x:i>
-      <x:x v="173"/>
-    </x:i>
-    <x:i>
-      <x:x v="174"/>
-    </x:i>
-    <x:i>
-      <x:x v="175"/>
-    </x:i>
-    <x:i>
-      <x:x v="176"/>
-    </x:i>
-    <x:i>
-      <x:x v="177"/>
-    </x:i>
-    <x:i>
-      <x:x v="178"/>
-    </x:i>
-    <x:i>
-      <x:x v="179"/>
-    </x:i>
-    <x:i>
-      <x:x v="180"/>
-    </x:i>
-    <x:i>
-      <x:x v="181"/>
-    </x:i>
-    <x:i>
-      <x:x v="182"/>
-    </x:i>
-    <x:i>
-      <x:x v="183"/>
-    </x:i>
-    <x:i>
-      <x:x v="184"/>
-    </x:i>
-    <x:i>
-      <x:x v="185"/>
-    </x:i>
-    <x:i>
-      <x:x v="186"/>
-    </x:i>
-    <x:i>
-      <x:x v="187"/>
-    </x:i>
-    <x:i>
-      <x:x v="188"/>
-    </x:i>
-    <x:i>
-      <x:x v="189"/>
-    </x:i>
-    <x:i>
-      <x:x v="190"/>
-    </x:i>
-    <x:i>
-      <x:x v="191"/>
-    </x:i>
-    <x:i>
-      <x:x v="192"/>
-    </x:i>
-    <x:i>
-      <x:x v="193"/>
-    </x:i>
-    <x:i>
-      <x:x v="194"/>
-    </x:i>
-    <x:i>
-      <x:x v="195"/>
-    </x:i>
-    <x:i>
-      <x:x v="196"/>
-    </x:i>
-    <x:i>
-      <x:x v="197"/>
-    </x:i>
-    <x:i>
-      <x:x v="198"/>
-    </x:i>
-    <x:i>
-      <x:x v="199"/>
-    </x:i>
-    <x:i>
-      <x:x v="200"/>
-    </x:i>
-    <x:i>
-      <x:x v="201"/>
-    </x:i>
-    <x:i>
-      <x:x v="202"/>
-    </x:i>
-    <x:i>
-      <x:x v="203"/>
-    </x:i>
-    <x:i>
-      <x:x v="204"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:rowItems>
-  <x:colFields count="2">
-    <x:field x="5"/>
-    <x:field x="-2"/>
-  </x:colFields>
-  <x:colItems count="4">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:colItems>
-  <x:dataFields count="2">
-    <x:dataField name="Sum Amount paid" fld="6" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Sum Items total" fld="4" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-  </x:dataFields>
-  <x:formats count="1">
-    <x:format dxfId="1">
-      <x:pivotArea type="normal" dataOnly="0" labelOnly="1" fieldPosition="0">
-        <x:references count="1">
-          <x:reference field="1"/>
-        </x:references>
-      </x:pivotArea>
-    </x:format>
-  </x:formats>
-  <x:pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
-    </x:ext>
-  </x:extLst>
-</x:pivotTableDefinition>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataPosition="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" itemPrintTitles="1" mergeItem="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1">
+  <location ref="B3:H9" firstHeaderRow="1" firstDataRow="3" firstDataCol="3"/>
+  <pivotFields count="7">
+    <pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="55">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Payment method" axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="206">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="145"/>
+        <item x="146"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="149"/>
+        <item x="150"/>
+        <item x="151"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="154"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="159"/>
+        <item x="160"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="163"/>
+        <item x="164"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="170"/>
+        <item x="171"/>
+        <item x="172"/>
+        <item x="173"/>
+        <item x="174"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="177"/>
+        <item x="178"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="182"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="185"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="190"/>
+        <item x="191"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="194"/>
+        <item x="195"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="198"/>
+        <item x="199"/>
+        <item x="200"/>
+        <item x="201"/>
+        <item x="202"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField name="Tax rate" axis="axisCol" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="0"/>
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <colFields count="2">
+    <field x="5"/>
+    <field x="-2"/>
+  </colFields>
+  <dataFields count="2">
+    <dataField name="Amount paid" fld="6"/>
+    <dataField name="Items total" fld="4"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition enableEdit="0" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" itemPrintTitles="1" mergeItem="1" indent="0" compact="0" compactData="0" gridDropZones="1">
-  <x:location ref="B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="7">
-    <x:pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0">
-      <x:items count="55">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item x="7"/>
-        <x:item x="8"/>
-        <x:item x="9"/>
-        <x:item x="10"/>
-        <x:item x="11"/>
-        <x:item x="12"/>
-        <x:item x="13"/>
-        <x:item x="14"/>
-        <x:item x="15"/>
-        <x:item x="16"/>
-        <x:item x="17"/>
-        <x:item x="18"/>
-        <x:item x="19"/>
-        <x:item x="20"/>
-        <x:item x="21"/>
-        <x:item x="22"/>
-        <x:item x="23"/>
-        <x:item x="24"/>
-        <x:item x="25"/>
-        <x:item x="26"/>
-        <x:item x="27"/>
-        <x:item x="28"/>
-        <x:item x="29"/>
-        <x:item x="30"/>
-        <x:item x="31"/>
-        <x:item x="32"/>
-        <x:item x="33"/>
-        <x:item x="34"/>
-        <x:item x="35"/>
-        <x:item x="36"/>
-        <x:item x="37"/>
-        <x:item x="38"/>
-        <x:item x="39"/>
-        <x:item x="40"/>
-        <x:item x="41"/>
-        <x:item x="42"/>
-        <x:item x="43"/>
-        <x:item x="44"/>
-        <x:item x="45"/>
-        <x:item x="46"/>
-        <x:item x="47"/>
-        <x:item x="48"/>
-        <x:item x="49"/>
-        <x:item x="50"/>
-        <x:item x="51"/>
-        <x:item x="52"/>
-        <x:item x="53"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Payment method" axis="axisCol" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="8">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
-      <x:items count="206">
-        <x:item x="0"/>
-        <x:item x="1"/>
-        <x:item x="2"/>
-        <x:item x="3"/>
-        <x:item x="4"/>
-        <x:item x="5"/>
-        <x:item x="6"/>
-        <x:item x="7"/>
-        <x:item x="8"/>
-        <x:item x="9"/>
-        <x:item x="10"/>
-        <x:item x="11"/>
-        <x:item x="12"/>
-        <x:item x="13"/>
-        <x:item x="14"/>
-        <x:item x="15"/>
-        <x:item x="16"/>
-        <x:item x="17"/>
-        <x:item x="18"/>
-        <x:item x="19"/>
-        <x:item x="20"/>
-        <x:item x="21"/>
-        <x:item x="22"/>
-        <x:item x="23"/>
-        <x:item x="24"/>
-        <x:item x="25"/>
-        <x:item x="26"/>
-        <x:item x="27"/>
-        <x:item x="28"/>
-        <x:item x="29"/>
-        <x:item x="30"/>
-        <x:item x="31"/>
-        <x:item x="32"/>
-        <x:item x="33"/>
-        <x:item x="34"/>
-        <x:item x="35"/>
-        <x:item x="36"/>
-        <x:item x="37"/>
-        <x:item x="38"/>
-        <x:item x="39"/>
-        <x:item x="40"/>
-        <x:item x="41"/>
-        <x:item x="42"/>
-        <x:item x="43"/>
-        <x:item x="44"/>
-        <x:item x="45"/>
-        <x:item x="46"/>
-        <x:item x="47"/>
-        <x:item x="48"/>
-        <x:item x="49"/>
-        <x:item x="50"/>
-        <x:item x="51"/>
-        <x:item x="52"/>
-        <x:item x="53"/>
-        <x:item x="54"/>
-        <x:item x="55"/>
-        <x:item x="56"/>
-        <x:item x="57"/>
-        <x:item x="58"/>
-        <x:item x="59"/>
-        <x:item x="60"/>
-        <x:item x="61"/>
-        <x:item x="62"/>
-        <x:item x="63"/>
-        <x:item x="64"/>
-        <x:item x="65"/>
-        <x:item x="66"/>
-        <x:item x="67"/>
-        <x:item x="68"/>
-        <x:item x="69"/>
-        <x:item x="70"/>
-        <x:item x="71"/>
-        <x:item x="72"/>
-        <x:item x="73"/>
-        <x:item x="74"/>
-        <x:item x="75"/>
-        <x:item x="76"/>
-        <x:item x="77"/>
-        <x:item x="78"/>
-        <x:item x="79"/>
-        <x:item x="80"/>
-        <x:item x="81"/>
-        <x:item x="82"/>
-        <x:item x="83"/>
-        <x:item x="84"/>
-        <x:item x="85"/>
-        <x:item x="86"/>
-        <x:item x="87"/>
-        <x:item x="88"/>
-        <x:item x="89"/>
-        <x:item x="90"/>
-        <x:item x="91"/>
-        <x:item x="92"/>
-        <x:item x="93"/>
-        <x:item x="94"/>
-        <x:item x="95"/>
-        <x:item x="96"/>
-        <x:item x="97"/>
-        <x:item x="98"/>
-        <x:item x="99"/>
-        <x:item x="100"/>
-        <x:item x="101"/>
-        <x:item x="102"/>
-        <x:item x="103"/>
-        <x:item x="104"/>
-        <x:item x="105"/>
-        <x:item x="106"/>
-        <x:item x="107"/>
-        <x:item x="108"/>
-        <x:item x="109"/>
-        <x:item x="110"/>
-        <x:item x="111"/>
-        <x:item x="112"/>
-        <x:item x="113"/>
-        <x:item x="114"/>
-        <x:item x="115"/>
-        <x:item x="116"/>
-        <x:item x="117"/>
-        <x:item x="118"/>
-        <x:item x="119"/>
-        <x:item x="120"/>
-        <x:item x="121"/>
-        <x:item x="122"/>
-        <x:item x="123"/>
-        <x:item x="124"/>
-        <x:item x="125"/>
-        <x:item x="126"/>
-        <x:item x="127"/>
-        <x:item x="128"/>
-        <x:item x="129"/>
-        <x:item x="130"/>
-        <x:item x="131"/>
-        <x:item x="132"/>
-        <x:item x="133"/>
-        <x:item x="134"/>
-        <x:item x="135"/>
-        <x:item x="136"/>
-        <x:item x="137"/>
-        <x:item x="138"/>
-        <x:item x="139"/>
-        <x:item x="140"/>
-        <x:item x="141"/>
-        <x:item x="142"/>
-        <x:item x="143"/>
-        <x:item x="144"/>
-        <x:item x="145"/>
-        <x:item x="146"/>
-        <x:item x="147"/>
-        <x:item x="148"/>
-        <x:item x="149"/>
-        <x:item x="150"/>
-        <x:item x="151"/>
-        <x:item x="152"/>
-        <x:item x="153"/>
-        <x:item x="154"/>
-        <x:item x="155"/>
-        <x:item x="156"/>
-        <x:item x="157"/>
-        <x:item x="158"/>
-        <x:item x="159"/>
-        <x:item x="160"/>
-        <x:item x="161"/>
-        <x:item x="162"/>
-        <x:item x="163"/>
-        <x:item x="164"/>
-        <x:item x="165"/>
-        <x:item x="166"/>
-        <x:item x="167"/>
-        <x:item x="168"/>
-        <x:item x="169"/>
-        <x:item x="170"/>
-        <x:item x="171"/>
-        <x:item x="172"/>
-        <x:item x="173"/>
-        <x:item x="174"/>
-        <x:item x="175"/>
-        <x:item x="176"/>
-        <x:item x="177"/>
-        <x:item x="178"/>
-        <x:item x="179"/>
-        <x:item x="180"/>
-        <x:item x="181"/>
-        <x:item x="182"/>
-        <x:item x="183"/>
-        <x:item x="184"/>
-        <x:item x="185"/>
-        <x:item x="186"/>
-        <x:item x="187"/>
-        <x:item x="188"/>
-        <x:item x="189"/>
-        <x:item x="190"/>
-        <x:item x="191"/>
-        <x:item x="192"/>
-        <x:item x="193"/>
-        <x:item x="194"/>
-        <x:item x="195"/>
-        <x:item x="196"/>
-        <x:item x="197"/>
-        <x:item x="198"/>
-        <x:item x="199"/>
-        <x:item x="200"/>
-        <x:item x="201"/>
-        <x:item x="202"/>
-        <x:item x="203"/>
-        <x:item x="204"/>
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Ship date" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Items total" dataField="1" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Tax rate" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Amount paid" compact="0" outline="0">
-      <x:items count="1">
-        <x:item t="default"/>
-      </x:items>
-    </x:pivotField>
-  </x:pivotFields>
-  <x:rowFields count="2">
-    <x:field x="0"/>
-    <x:field x="2"/>
-  </x:rowFields>
-  <x:rowItems count="261">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i>
-      <x:x v="5"/>
-    </x:i>
-    <x:i>
-      <x:x v="6"/>
-    </x:i>
-    <x:i>
-      <x:x v="7"/>
-    </x:i>
-    <x:i>
-      <x:x v="8"/>
-    </x:i>
-    <x:i>
-      <x:x v="9"/>
-    </x:i>
-    <x:i>
-      <x:x v="10"/>
-    </x:i>
-    <x:i>
-      <x:x v="11"/>
-    </x:i>
-    <x:i>
-      <x:x v="12"/>
-    </x:i>
-    <x:i>
-      <x:x v="13"/>
-    </x:i>
-    <x:i>
-      <x:x v="14"/>
-    </x:i>
-    <x:i>
-      <x:x v="15"/>
-    </x:i>
-    <x:i>
-      <x:x v="16"/>
-    </x:i>
-    <x:i>
-      <x:x v="17"/>
-    </x:i>
-    <x:i>
-      <x:x v="18"/>
-    </x:i>
-    <x:i>
-      <x:x v="19"/>
-    </x:i>
-    <x:i>
-      <x:x v="20"/>
-    </x:i>
-    <x:i>
-      <x:x v="21"/>
-    </x:i>
-    <x:i>
-      <x:x v="22"/>
-    </x:i>
-    <x:i>
-      <x:x v="23"/>
-    </x:i>
-    <x:i>
-      <x:x v="24"/>
-    </x:i>
-    <x:i>
-      <x:x v="25"/>
-    </x:i>
-    <x:i>
-      <x:x v="26"/>
-    </x:i>
-    <x:i>
-      <x:x v="27"/>
-    </x:i>
-    <x:i>
-      <x:x v="28"/>
-    </x:i>
-    <x:i>
-      <x:x v="29"/>
-    </x:i>
-    <x:i>
-      <x:x v="30"/>
-    </x:i>
-    <x:i>
-      <x:x v="31"/>
-    </x:i>
-    <x:i>
-      <x:x v="32"/>
-    </x:i>
-    <x:i>
-      <x:x v="33"/>
-    </x:i>
-    <x:i>
-      <x:x v="34"/>
-    </x:i>
-    <x:i>
-      <x:x v="35"/>
-    </x:i>
-    <x:i>
-      <x:x v="36"/>
-    </x:i>
-    <x:i>
-      <x:x v="37"/>
-    </x:i>
-    <x:i>
-      <x:x v="38"/>
-    </x:i>
-    <x:i>
-      <x:x v="39"/>
-    </x:i>
-    <x:i>
-      <x:x v="40"/>
-    </x:i>
-    <x:i>
-      <x:x v="41"/>
-    </x:i>
-    <x:i>
-      <x:x v="42"/>
-    </x:i>
-    <x:i>
-      <x:x v="43"/>
-    </x:i>
-    <x:i>
-      <x:x v="44"/>
-    </x:i>
-    <x:i>
-      <x:x v="45"/>
-    </x:i>
-    <x:i>
-      <x:x v="46"/>
-    </x:i>
-    <x:i>
-      <x:x v="47"/>
-    </x:i>
-    <x:i>
-      <x:x v="48"/>
-    </x:i>
-    <x:i>
-      <x:x v="49"/>
-    </x:i>
-    <x:i>
-      <x:x v="50"/>
-    </x:i>
-    <x:i>
-      <x:x v="51"/>
-    </x:i>
-    <x:i>
-      <x:x v="52"/>
-    </x:i>
-    <x:i>
-      <x:x v="53"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i>
-      <x:x v="5"/>
-    </x:i>
-    <x:i>
-      <x:x v="6"/>
-    </x:i>
-    <x:i>
-      <x:x v="7"/>
-    </x:i>
-    <x:i>
-      <x:x v="8"/>
-    </x:i>
-    <x:i>
-      <x:x v="9"/>
-    </x:i>
-    <x:i>
-      <x:x v="10"/>
-    </x:i>
-    <x:i>
-      <x:x v="11"/>
-    </x:i>
-    <x:i>
-      <x:x v="12"/>
-    </x:i>
-    <x:i>
-      <x:x v="13"/>
-    </x:i>
-    <x:i>
-      <x:x v="14"/>
-    </x:i>
-    <x:i>
-      <x:x v="15"/>
-    </x:i>
-    <x:i>
-      <x:x v="16"/>
-    </x:i>
-    <x:i>
-      <x:x v="17"/>
-    </x:i>
-    <x:i>
-      <x:x v="18"/>
-    </x:i>
-    <x:i>
-      <x:x v="19"/>
-    </x:i>
-    <x:i>
-      <x:x v="20"/>
-    </x:i>
-    <x:i>
-      <x:x v="21"/>
-    </x:i>
-    <x:i>
-      <x:x v="22"/>
-    </x:i>
-    <x:i>
-      <x:x v="23"/>
-    </x:i>
-    <x:i>
-      <x:x v="24"/>
-    </x:i>
-    <x:i>
-      <x:x v="25"/>
-    </x:i>
-    <x:i>
-      <x:x v="26"/>
-    </x:i>
-    <x:i>
-      <x:x v="27"/>
-    </x:i>
-    <x:i>
-      <x:x v="28"/>
-    </x:i>
-    <x:i>
-      <x:x v="29"/>
-    </x:i>
-    <x:i>
-      <x:x v="30"/>
-    </x:i>
-    <x:i>
-      <x:x v="31"/>
-    </x:i>
-    <x:i>
-      <x:x v="32"/>
-    </x:i>
-    <x:i>
-      <x:x v="33"/>
-    </x:i>
-    <x:i>
-      <x:x v="34"/>
-    </x:i>
-    <x:i>
-      <x:x v="35"/>
-    </x:i>
-    <x:i>
-      <x:x v="36"/>
-    </x:i>
-    <x:i>
-      <x:x v="37"/>
-    </x:i>
-    <x:i>
-      <x:x v="38"/>
-    </x:i>
-    <x:i>
-      <x:x v="39"/>
-    </x:i>
-    <x:i>
-      <x:x v="40"/>
-    </x:i>
-    <x:i>
-      <x:x v="41"/>
-    </x:i>
-    <x:i>
-      <x:x v="42"/>
-    </x:i>
-    <x:i>
-      <x:x v="43"/>
-    </x:i>
-    <x:i>
-      <x:x v="44"/>
-    </x:i>
-    <x:i>
-      <x:x v="45"/>
-    </x:i>
-    <x:i>
-      <x:x v="46"/>
-    </x:i>
-    <x:i>
-      <x:x v="47"/>
-    </x:i>
-    <x:i>
-      <x:x v="48"/>
-    </x:i>
-    <x:i>
-      <x:x v="49"/>
-    </x:i>
-    <x:i>
-      <x:x v="50"/>
-    </x:i>
-    <x:i>
-      <x:x v="51"/>
-    </x:i>
-    <x:i>
-      <x:x v="52"/>
-    </x:i>
-    <x:i>
-      <x:x v="53"/>
-    </x:i>
-    <x:i>
-      <x:x v="54"/>
-    </x:i>
-    <x:i>
-      <x:x v="55"/>
-    </x:i>
-    <x:i>
-      <x:x v="56"/>
-    </x:i>
-    <x:i>
-      <x:x v="57"/>
-    </x:i>
-    <x:i>
-      <x:x v="58"/>
-    </x:i>
-    <x:i>
-      <x:x v="59"/>
-    </x:i>
-    <x:i>
-      <x:x v="60"/>
-    </x:i>
-    <x:i>
-      <x:x v="61"/>
-    </x:i>
-    <x:i>
-      <x:x v="62"/>
-    </x:i>
-    <x:i>
-      <x:x v="63"/>
-    </x:i>
-    <x:i>
-      <x:x v="64"/>
-    </x:i>
-    <x:i>
-      <x:x v="65"/>
-    </x:i>
-    <x:i>
-      <x:x v="66"/>
-    </x:i>
-    <x:i>
-      <x:x v="67"/>
-    </x:i>
-    <x:i>
-      <x:x v="68"/>
-    </x:i>
-    <x:i>
-      <x:x v="69"/>
-    </x:i>
-    <x:i>
-      <x:x v="70"/>
-    </x:i>
-    <x:i>
-      <x:x v="71"/>
-    </x:i>
-    <x:i>
-      <x:x v="72"/>
-    </x:i>
-    <x:i>
-      <x:x v="73"/>
-    </x:i>
-    <x:i>
-      <x:x v="74"/>
-    </x:i>
-    <x:i>
-      <x:x v="75"/>
-    </x:i>
-    <x:i>
-      <x:x v="76"/>
-    </x:i>
-    <x:i>
-      <x:x v="77"/>
-    </x:i>
-    <x:i>
-      <x:x v="78"/>
-    </x:i>
-    <x:i>
-      <x:x v="79"/>
-    </x:i>
-    <x:i>
-      <x:x v="80"/>
-    </x:i>
-    <x:i>
-      <x:x v="81"/>
-    </x:i>
-    <x:i>
-      <x:x v="82"/>
-    </x:i>
-    <x:i>
-      <x:x v="83"/>
-    </x:i>
-    <x:i>
-      <x:x v="84"/>
-    </x:i>
-    <x:i>
-      <x:x v="85"/>
-    </x:i>
-    <x:i>
-      <x:x v="86"/>
-    </x:i>
-    <x:i>
-      <x:x v="87"/>
-    </x:i>
-    <x:i>
-      <x:x v="88"/>
-    </x:i>
-    <x:i>
-      <x:x v="89"/>
-    </x:i>
-    <x:i>
-      <x:x v="90"/>
-    </x:i>
-    <x:i>
-      <x:x v="91"/>
-    </x:i>
-    <x:i>
-      <x:x v="92"/>
-    </x:i>
-    <x:i>
-      <x:x v="93"/>
-    </x:i>
-    <x:i>
-      <x:x v="94"/>
-    </x:i>
-    <x:i>
-      <x:x v="95"/>
-    </x:i>
-    <x:i>
-      <x:x v="96"/>
-    </x:i>
-    <x:i>
-      <x:x v="97"/>
-    </x:i>
-    <x:i>
-      <x:x v="98"/>
-    </x:i>
-    <x:i>
-      <x:x v="99"/>
-    </x:i>
-    <x:i>
-      <x:x v="100"/>
-    </x:i>
-    <x:i>
-      <x:x v="101"/>
-    </x:i>
-    <x:i>
-      <x:x v="102"/>
-    </x:i>
-    <x:i>
-      <x:x v="103"/>
-    </x:i>
-    <x:i>
-      <x:x v="104"/>
-    </x:i>
-    <x:i>
-      <x:x v="105"/>
-    </x:i>
-    <x:i>
-      <x:x v="106"/>
-    </x:i>
-    <x:i>
-      <x:x v="107"/>
-    </x:i>
-    <x:i>
-      <x:x v="108"/>
-    </x:i>
-    <x:i>
-      <x:x v="109"/>
-    </x:i>
-    <x:i>
-      <x:x v="110"/>
-    </x:i>
-    <x:i>
-      <x:x v="111"/>
-    </x:i>
-    <x:i>
-      <x:x v="112"/>
-    </x:i>
-    <x:i>
-      <x:x v="113"/>
-    </x:i>
-    <x:i>
-      <x:x v="114"/>
-    </x:i>
-    <x:i>
-      <x:x v="115"/>
-    </x:i>
-    <x:i>
-      <x:x v="116"/>
-    </x:i>
-    <x:i>
-      <x:x v="117"/>
-    </x:i>
-    <x:i>
-      <x:x v="118"/>
-    </x:i>
-    <x:i>
-      <x:x v="119"/>
-    </x:i>
-    <x:i>
-      <x:x v="120"/>
-    </x:i>
-    <x:i>
-      <x:x v="121"/>
-    </x:i>
-    <x:i>
-      <x:x v="122"/>
-    </x:i>
-    <x:i>
-      <x:x v="123"/>
-    </x:i>
-    <x:i>
-      <x:x v="124"/>
-    </x:i>
-    <x:i>
-      <x:x v="125"/>
-    </x:i>
-    <x:i>
-      <x:x v="126"/>
-    </x:i>
-    <x:i>
-      <x:x v="127"/>
-    </x:i>
-    <x:i>
-      <x:x v="128"/>
-    </x:i>
-    <x:i>
-      <x:x v="129"/>
-    </x:i>
-    <x:i>
-      <x:x v="130"/>
-    </x:i>
-    <x:i>
-      <x:x v="131"/>
-    </x:i>
-    <x:i>
-      <x:x v="132"/>
-    </x:i>
-    <x:i>
-      <x:x v="133"/>
-    </x:i>
-    <x:i>
-      <x:x v="134"/>
-    </x:i>
-    <x:i>
-      <x:x v="135"/>
-    </x:i>
-    <x:i>
-      <x:x v="136"/>
-    </x:i>
-    <x:i>
-      <x:x v="137"/>
-    </x:i>
-    <x:i>
-      <x:x v="138"/>
-    </x:i>
-    <x:i>
-      <x:x v="139"/>
-    </x:i>
-    <x:i>
-      <x:x v="140"/>
-    </x:i>
-    <x:i>
-      <x:x v="141"/>
-    </x:i>
-    <x:i>
-      <x:x v="142"/>
-    </x:i>
-    <x:i>
-      <x:x v="143"/>
-    </x:i>
-    <x:i>
-      <x:x v="144"/>
-    </x:i>
-    <x:i>
-      <x:x v="145"/>
-    </x:i>
-    <x:i>
-      <x:x v="146"/>
-    </x:i>
-    <x:i>
-      <x:x v="147"/>
-    </x:i>
-    <x:i>
-      <x:x v="148"/>
-    </x:i>
-    <x:i>
-      <x:x v="149"/>
-    </x:i>
-    <x:i>
-      <x:x v="150"/>
-    </x:i>
-    <x:i>
-      <x:x v="151"/>
-    </x:i>
-    <x:i>
-      <x:x v="152"/>
-    </x:i>
-    <x:i>
-      <x:x v="153"/>
-    </x:i>
-    <x:i>
-      <x:x v="154"/>
-    </x:i>
-    <x:i>
-      <x:x v="155"/>
-    </x:i>
-    <x:i>
-      <x:x v="156"/>
-    </x:i>
-    <x:i>
-      <x:x v="157"/>
-    </x:i>
-    <x:i>
-      <x:x v="158"/>
-    </x:i>
-    <x:i>
-      <x:x v="159"/>
-    </x:i>
-    <x:i>
-      <x:x v="160"/>
-    </x:i>
-    <x:i>
-      <x:x v="161"/>
-    </x:i>
-    <x:i>
-      <x:x v="162"/>
-    </x:i>
-    <x:i>
-      <x:x v="163"/>
-    </x:i>
-    <x:i>
-      <x:x v="164"/>
-    </x:i>
-    <x:i>
-      <x:x v="165"/>
-    </x:i>
-    <x:i>
-      <x:x v="166"/>
-    </x:i>
-    <x:i>
-      <x:x v="167"/>
-    </x:i>
-    <x:i>
-      <x:x v="168"/>
-    </x:i>
-    <x:i>
-      <x:x v="169"/>
-    </x:i>
-    <x:i>
-      <x:x v="170"/>
-    </x:i>
-    <x:i>
-      <x:x v="171"/>
-    </x:i>
-    <x:i>
-      <x:x v="172"/>
-    </x:i>
-    <x:i>
-      <x:x v="173"/>
-    </x:i>
-    <x:i>
-      <x:x v="174"/>
-    </x:i>
-    <x:i>
-      <x:x v="175"/>
-    </x:i>
-    <x:i>
-      <x:x v="176"/>
-    </x:i>
-    <x:i>
-      <x:x v="177"/>
-    </x:i>
-    <x:i>
-      <x:x v="178"/>
-    </x:i>
-    <x:i>
-      <x:x v="179"/>
-    </x:i>
-    <x:i>
-      <x:x v="180"/>
-    </x:i>
-    <x:i>
-      <x:x v="181"/>
-    </x:i>
-    <x:i>
-      <x:x v="182"/>
-    </x:i>
-    <x:i>
-      <x:x v="183"/>
-    </x:i>
-    <x:i>
-      <x:x v="184"/>
-    </x:i>
-    <x:i>
-      <x:x v="185"/>
-    </x:i>
-    <x:i>
-      <x:x v="186"/>
-    </x:i>
-    <x:i>
-      <x:x v="187"/>
-    </x:i>
-    <x:i>
-      <x:x v="188"/>
-    </x:i>
-    <x:i>
-      <x:x v="189"/>
-    </x:i>
-    <x:i>
-      <x:x v="190"/>
-    </x:i>
-    <x:i>
-      <x:x v="191"/>
-    </x:i>
-    <x:i>
-      <x:x v="192"/>
-    </x:i>
-    <x:i>
-      <x:x v="193"/>
-    </x:i>
-    <x:i>
-      <x:x v="194"/>
-    </x:i>
-    <x:i>
-      <x:x v="195"/>
-    </x:i>
-    <x:i>
-      <x:x v="196"/>
-    </x:i>
-    <x:i>
-      <x:x v="197"/>
-    </x:i>
-    <x:i>
-      <x:x v="198"/>
-    </x:i>
-    <x:i>
-      <x:x v="199"/>
-    </x:i>
-    <x:i>
-      <x:x v="200"/>
-    </x:i>
-    <x:i>
-      <x:x v="201"/>
-    </x:i>
-    <x:i>
-      <x:x v="202"/>
-    </x:i>
-    <x:i>
-      <x:x v="203"/>
-    </x:i>
-    <x:i>
-      <x:x v="204"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:rowItems>
-  <x:colFields count="1">
-    <x:field x="1"/>
-  </x:colFields>
-  <x:colItems count="8">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i>
-      <x:x v="1"/>
-    </x:i>
-    <x:i>
-      <x:x v="2"/>
-    </x:i>
-    <x:i>
-      <x:x v="3"/>
-    </x:i>
-    <x:i>
-      <x:x v="4"/>
-    </x:i>
-    <x:i>
-      <x:x v="5"/>
-    </x:i>
-    <x:i>
-      <x:x v="6"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:colItems>
-  <x:dataFields count="1">
-    <x:dataField name="Sum of Items total" fld="4" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
-  </x:dataFields>
-  <x:formats count="1">
-    <x:format dxfId="1">
-      <x:pivotArea type="normal" dataOnly="0" labelOnly="1" fieldPosition="0">
-        <x:references count="1">
-          <x:reference field="1"/>
-        </x:references>
-      </x:pivotArea>
-    </x:format>
-  </x:formats>
-  <x:pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
-    </x:ext>
-  </x:extLst>
-</x:pivotTableDefinition>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" mergeItem="1" createdVersion="3" indent="0" compact="0" compactData="0" gridDropZones="1">
+  <location ref="B4:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
+  <pivotFields count="7">
+    <pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="55">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Payment method" axis="axisCol" compact="0" outline="0" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="206">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="145"/>
+        <item x="146"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="149"/>
+        <item x="150"/>
+        <item x="151"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="154"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="159"/>
+        <item x="160"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="163"/>
+        <item x="164"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="170"/>
+        <item x="171"/>
+        <item x="172"/>
+        <item x="173"/>
+        <item x="174"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="177"/>
+        <item x="178"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="182"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="185"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="190"/>
+        <item x="191"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="194"/>
+        <item x="195"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="198"/>
+        <item x="199"/>
+        <item x="200"/>
+        <item x="201"/>
+        <item x="202"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="2"/>
+  </rowFields>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <dataFields count="1">
+    <dataField name="Items total" fld="4"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition enableEdit="0" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>